<commit_message>
Saved for the Week off
</commit_message>
<xml_diff>
--- a/CurrentStressEquations.xlsx
+++ b/CurrentStressEquations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.sfwmd.gov\dfsroot\data\wsd\SUP\proj\CFWI_WetlandStress\Update2018\EvalCurrentStress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD17E4C6-29AF-4B75-AC99-54ADAE9F2F79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7461DCF6-8A3B-45EE-BA25-A40E5BCA85E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1650" windowWidth="23805" windowHeight="13110" xr2:uid="{610297E1-C0D6-4F00-8E4F-2F0A7D67BC3D}"/>
+    <workbookView xWindow="29475" yWindow="1545" windowWidth="23805" windowHeight="13110" xr2:uid="{610297E1-C0D6-4F00-8E4F-2F0A7D67BC3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>Stressed Plain Wetlands</t>
   </si>
@@ -101,13 +101,98 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shapiro.test for </t>
+  </si>
+  <si>
+    <t>Not Stressed</t>
+  </si>
+  <si>
+    <t>Plain</t>
+  </si>
+  <si>
+    <t>Stressed</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>C1[C1$Phys=="Ridge",]$SimEpsilon&lt;-C1[C1$Phys=="Ridge",]$AreaWgtp05L1-C1[C1$Phys=="Ridge",]$AreaWgtp80L1
+C1[C1$Phys=="Plain",]$SimEpsilon&lt;-C1[C1$Phys=="Plain",]$AreaWgtp05L1-C1[C1$Phys=="Plain",]$AreaWgtp80L1</t>
+  </si>
+  <si>
+    <r>
+      <t>C1[C1$Phys=="Ridge",]$SimEpsilon&lt;-C1[C1$Phys=="Ridge",]$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AreaWgtp05L3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-C1[C1$Phys=="Ridge",]$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AreaWgtp80L3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C1[C1$Phys=="Plain",]$SimEpsilon&lt;-C1[C1$Phys=="Plain",]$AreaWgtp05L1-C1[C1$Phys=="Plain",]$AreaWgtp80L1</t>
+    </r>
+  </si>
+  <si>
+    <t>C1[C1$Phys=="Ridge",]$SimEpsilon&lt;-C1[C1$Phys=="Ridge",]$AreaWgtp05L1-C1[C1$Phys=="Ridge",]$AreaWgtp80L1
+C1[C1$Phys=="Plain", ]$SimEpsilon&lt;-C1[C1$Phys=="Plain", ]$AreaWgtp05L1-C1[C1$Phys=="Plain", ]$AreaWgtp80L1</t>
+  </si>
+  <si>
+    <t>C1[C1$Phys=="Ridge",]$SimEpsilon&lt;-C1[C1$Phys=="Ridge",]$AreaWgttopo-C1[C1$Phys=="Ridge",]$AreaWgtp80L1
+C1[C1$Phys=="Plain",]$SimEpsilon&lt;-C1[C1$Phys=="Plain",]$AreaWgttopo-C1[C1$Phys=="Plain",]$AreaWgtp80L1</t>
+  </si>
+  <si>
+    <t>L1P05  -L1P80 plain L3P05 - L3P80 ridge  Stress Periods 1-25</t>
+  </si>
+  <si>
+    <t>Model topo - L1P80 Stress Periods 1-25</t>
+  </si>
+  <si>
+    <t>L1P05  -L1P80 plain L1P05 - L1P80 ridge  Stress Periods 1-25</t>
+  </si>
+  <si>
+    <t>L1P05  -L1P80 plain L1P05 - L1P80 ridge  Full POR 1-133</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,13 +207,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,10 +268,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,8 +281,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -173,15 +319,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4359728</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -221,8 +367,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6858000" y="190500"/>
-          <a:ext cx="2514600" cy="800100"/>
+          <a:off x="7629525" y="257175"/>
+          <a:ext cx="3797753" cy="942975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -612,17 +758,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B067AB78-D6BE-42E9-8E00-79354997FF63}">
-  <dimension ref="B1:I15"/>
+  <dimension ref="B1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="10" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="107.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -819,6 +969,406 @@
       <c r="E15" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="F18" t="str">
+        <f>CHAR(13)</f>
+        <v>_x000D_</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="E19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>0.95620000000000005</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1.18E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>0.95930000000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.14860000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>0.95020000000000004</v>
+      </c>
+      <c r="G22">
+        <v>0.11459999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="G23">
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="E25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>0.96650000000000003</v>
+      </c>
+      <c r="G26">
+        <v>5.1900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>0.97950000000000004</v>
+      </c>
+      <c r="G27">
+        <v>0.64280000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>0.95689999999999997</v>
+      </c>
+      <c r="G28">
+        <v>0.1721</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>0.96830000000000005</v>
+      </c>
+      <c r="G29">
+        <v>0.38129999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="E31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>73</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32">
+        <v>0.96650000000000003</v>
+      </c>
+      <c r="G32">
+        <v>5.1900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>0.97950000000000004</v>
+      </c>
+      <c r="G33">
+        <v>0.64280000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="G34" s="7">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35">
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="G35">
+        <v>0.1197</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="E37" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38">
+        <v>0.97009999999999996</v>
+      </c>
+      <c r="G38">
+        <v>7.6700000000000004E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39">
+        <v>0.92620000000000002</v>
+      </c>
+      <c r="G39" s="7">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40">
+        <v>0.93920000000000003</v>
+      </c>
+      <c r="G40" s="7">
+        <v>4.7800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41">
+        <v>0.96330000000000005</v>
+      </c>
+      <c r="G41">
+        <v>0.27150000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>